<commit_message>
next push from 2th feb 2024
</commit_message>
<xml_diff>
--- a/QA_Legend/src/main/java/testData/testData_Excel.xlsx
+++ b/QA_Legend/src/main/java/testData/testData_Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAUMIA\eclipse-workspace\QA_Legend\src\main\java\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAUMIA\git\JenkinsRepo\QA_Legend\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A09BF99-5464-4369-BEB6-65ACE8064810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1536CF3-6152-432B-950A-163447FB56E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Title</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>endDate</t>
+  </si>
+  <si>
+    <t>ItemQuantity</t>
+  </si>
+  <si>
+    <t>Rate</t>
   </si>
 </sst>
 </file>
@@ -581,14 +587,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1787B36E-1EDF-48B9-8C10-FABE8669726C}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -611,6 +618,22 @@
       </c>
       <c r="B3">
         <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -687,7 +710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AB3388-3C53-4D6D-934C-D6583694972B}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
QALegend push from 8th feb 2024
</commit_message>
<xml_diff>
--- a/QA_Legend/src/main/java/testData/testData_Excel.xlsx
+++ b/QA_Legend/src/main/java/testData/testData_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAUMIA\git\JenkinsRepo\QA_Legend\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1536CF3-6152-432B-950A-163447FB56E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812FB32F-8E38-4C79-936A-F48CAA102CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="LeavePage" sheetId="3" r:id="rId3"/>
     <sheet name="TaskPage" sheetId="4" r:id="rId4"/>
     <sheet name="InvoicePage" sheetId="5" r:id="rId5"/>
-    <sheet name="TeamMembers" sheetId="6" r:id="rId6"/>
-    <sheet name="Announcements" sheetId="7" r:id="rId7"/>
+    <sheet name="MessagePage" sheetId="8" r:id="rId6"/>
+    <sheet name="TeamMembers" sheetId="6" r:id="rId7"/>
+    <sheet name="Announcements" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>Title</t>
   </si>
@@ -124,6 +125,18 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>TestSubject</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>TestMessage</t>
   </si>
 </sst>
 </file>
@@ -589,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1787B36E-1EDF-48B9-8C10-FABE8669726C}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -643,6 +656,37 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0ACFF8C-7920-4D7E-9E8C-CD3873F9BC38}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E959E7E1-53B8-4AD1-953C-A3BDC7383A87}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -706,7 +750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AB3388-3C53-4D6D-934C-D6583694972B}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>

<commit_message>
commit 10 feb 2024
</commit_message>
<xml_diff>
--- a/QA_Legend/src/main/java/testData/testData_Excel.xlsx
+++ b/QA_Legend/src/main/java/testData/testData_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAUMIA\git\JenkinsRepo\QA_Legend\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812FB32F-8E38-4C79-936A-F48CAA102CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A91BB2-70E8-4D77-A628-1980B4FE8495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,10 @@
     <sheet name="TaskPage" sheetId="4" r:id="rId4"/>
     <sheet name="InvoicePage" sheetId="5" r:id="rId5"/>
     <sheet name="MessagePage" sheetId="8" r:id="rId6"/>
-    <sheet name="TeamMembers" sheetId="6" r:id="rId7"/>
-    <sheet name="Announcements" sheetId="7" r:id="rId8"/>
+    <sheet name="TicketsPage" sheetId="9" r:id="rId7"/>
+    <sheet name="LoginPage" sheetId="10" r:id="rId8"/>
+    <sheet name="TeamMembers" sheetId="6" r:id="rId9"/>
+    <sheet name="Announcements" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Title</t>
   </si>
@@ -137,6 +139,30 @@
   </si>
   <si>
     <t>TestMessage</t>
+  </si>
+  <si>
+    <t>Test Title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>admin@admin.com</t>
+  </si>
+  <si>
+    <t>saumiaalex@mailinator.com</t>
+  </si>
+  <si>
+    <t>Saumia@123</t>
+  </si>
+  <si>
+    <t>fakeuser@mailinator.com</t>
+  </si>
+  <si>
+    <t>fakePassword</t>
   </si>
 </sst>
 </file>
@@ -503,6 +529,48 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AB3388-3C53-4D6D-934C-D6583694972B}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="2">
+        <v>45567</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D8CE8A-3D14-4F85-B99D-46B868066EB7}">
   <dimension ref="A1:B1"/>
@@ -659,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0ACFF8C-7920-4D7E-9E8C-CD3873F9BC38}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -687,6 +755,102 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09DBEDD9-3EB3-4550-9411-489BBBB1A3E5}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59693EC-8028-46EE-93CB-21ED5D5C1CA7}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2">
+        <v>12345678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{C65567D8-78CB-442E-8BBE-FAADD6F49067}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{8014D698-DC58-4118-A2E7-093D3CEAD210}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{0E0C08AC-D3ED-4F7D-8398-0315B667199A}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{1DC4ACA7-5340-4935-8B97-A20033D512B0}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{06AFB774-8A85-4516-A700-6DFF48C5B191}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E959E7E1-53B8-4AD1-953C-A3BDC7383A87}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -748,46 +912,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35AB3388-3C53-4D6D-934C-D6583694972B}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2">
-        <v>45445</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="2">
-        <v>45567</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Uncommented all testcases in testng and rectified the error in add invoice
</commit_message>
<xml_diff>
--- a/QA_Legend/src/main/java/testData/testData_Excel.xlsx
+++ b/QA_Legend/src/main/java/testData/testData_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAUMIA\git\JenkinsRepo\QA_Legend\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A91BB2-70E8-4D77-A628-1980B4FE8495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B797E149-141D-4C12-A7C3-9906EAAD8E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Title</t>
   </si>
@@ -153,16 +153,13 @@
     <t>admin@admin.com</t>
   </si>
   <si>
-    <t>saumiaalex@mailinator.com</t>
-  </si>
-  <si>
-    <t>Saumia@123</t>
-  </si>
-  <si>
-    <t>fakeuser@mailinator.com</t>
-  </si>
-  <si>
     <t>fakePassword</t>
+  </si>
+  <si>
+    <t>fakeid@fake.com</t>
+  </si>
+  <si>
+    <t>fake@password</t>
   </si>
 </sst>
 </file>
@@ -790,12 +787,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -816,35 +814,35 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
         <v>39</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>12345678</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{C65567D8-78CB-442E-8BBE-FAADD6F49067}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{8014D698-DC58-4118-A2E7-093D3CEAD210}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{0E0C08AC-D3ED-4F7D-8398-0315B667199A}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{1DC4ACA7-5340-4935-8B97-A20033D512B0}"/>
-    <hyperlink ref="A4" r:id="rId5" xr:uid="{06AFB774-8A85-4516-A700-6DFF48C5B191}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{8014D698-DC58-4118-A2E7-093D3CEAD210}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{0E0C08AC-D3ED-4F7D-8398-0315B667199A}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{789024FA-3C03-4FF8-ABB7-54A1426FD2DA}"/>
+    <hyperlink ref="A4" r:id="rId5" xr:uid="{1D728DBD-BEC5-48F1-B9D0-3B33DCDEEBCF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>